<commit_message>
Updated Ch. 2.2,3,4, Ch. 3
Added usage data
</commit_message>
<xml_diff>
--- a/Appendix1/chv-report-june-2013.xlsx
+++ b/Appendix1/chv-report-june-2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>Adolescent and youth - Girls (13-24 yrs)</t>
   </si>
@@ -172,6 +172,57 @@
   </si>
   <si>
     <t>Maternal deaths</t>
+  </si>
+  <si>
+    <t>Pregnant women who did not attend 4 ANC visits</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Quality of Work Life</t>
+  </si>
+  <si>
+    <t>Perceived Ease of Use</t>
+  </si>
+  <si>
+    <t>Perceived Usefulness</t>
+  </si>
+  <si>
+    <t>User Control</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. The system helps me to do my job as a CHV better. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. I find the Baby Monitor system easy to use. </t>
+  </si>
+  <si>
+    <t>2. It is easy to report a home visit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. It is easy to report a delivery. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. It is easy to report an emergency. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. I like receiving SMS messages from Baby Monitor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. The messages help me keep track of my clients. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. The Baby Monitor system saves me time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. The messages that the Baby Monitor sends me are easy to understand. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. The messages are usually accurate. </t>
   </si>
 </sst>
 </file>
@@ -613,7 +664,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -625,6 +676,26 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="38" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="2"/>
@@ -972,7 +1043,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1743,7 @@
     <col min="1" max="1" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1680,135 +1751,105 @@
         <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="7">
         <v>148</v>
       </c>
-      <c r="C2" s="7">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="C2" s="6">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="7">
         <v>22</v>
       </c>
-      <c r="C3" s="7">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B4" s="7">
         <v>19</v>
       </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="7">
         <v>15</v>
       </c>
-      <c r="C5" s="7">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="7">
         <v>11</v>
       </c>
-      <c r="C6" s="7">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C6" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="7">
         <v>30</v>
       </c>
-      <c r="C7" s="7">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="C7" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="7">
         <v>17</v>
       </c>
-      <c r="C8" s="7">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="7">
         <v>58</v>
       </c>
-      <c r="C9" s="7">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="C9" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="7">
         <v>0</v>
       </c>
-      <c r="C10" s="7">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1819,12 +1860,113 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>